<commit_message>
update tuolumne drought logic
</commit_message>
<xml_diff>
--- a/preprocessing/other/USGS Gauge Flow Data extraction/USGS gauges.xlsx
+++ b/preprocessing/other/USGS Gauge Flow Data extraction/USGS gauges.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\PROJECTS\SIERRA2\Pywr models\preprocessing\USGS Gauge Flow Data extraction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\PROJECTS\SIERRA2\Pywr models\preprocessing\other\USGS Gauge Flow Data extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD4C9F0-1A75-43DA-A330-983D7DA3BC57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C525DC-7A09-4317-AE10-5154EACC4C68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merced - streamflow" sheetId="1" r:id="rId1"/>
@@ -1028,7 +1028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AEE754-2BE5-4781-AA16-1F6A506BBE5E}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1521,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E79526-C442-483C-B085-96826ED95061}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>